<commit_message>
income statement logo and sumbit issue
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test2.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test2.xlsx
@@ -322,9 +322,6 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -392,6 +389,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -478,6 +478,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>501150</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>73340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4730393" y="10884185"/>
+          <a:ext cx="2170701" cy="929520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,730 +792,730 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="89.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
-    <col min="9" max="1024" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="89.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
+    <col min="9" max="1024" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="3" customFormat="1" ht="45.95" customHeight="1">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
+    <row r="1" spans="2:17" s="2" customFormat="1" ht="45.95" customHeight="1">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="2:17" ht="1.5" customHeight="1">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>2018</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>2019</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>2020</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>10000</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>15000</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>15000</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>5500</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>7500</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>7500</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11">
-        <v>0</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f>SUM(C4:C8)</f>
         <v>15500</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <f>SUM(D4:D8)</f>
         <v>22500</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <f>SUM(E4:E8)</f>
         <v>22500</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="11.1" customHeight="1">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>2018</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>2019</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>2020</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>500</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>450</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>450</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11">
-        <v>0</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="11">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>5500</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>7500</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>7500</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="21.95" customHeight="1">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="11">
-        <v>0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="11">
-        <v>0</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="11">
-        <v>0</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="11">
-        <v>0</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="11">
-        <v>0</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="11">
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="11">
-        <v>0</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0</v>
-      </c>
-      <c r="E22" s="11">
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="11">
-        <v>0</v>
-      </c>
-      <c r="E23" s="11">
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="11">
-        <v>0</v>
-      </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="11">
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="11">
-        <v>0</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11">
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>6500</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>8500</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>8500</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11">
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="11">
-        <v>0</v>
-      </c>
-      <c r="D28" s="11">
-        <v>0</v>
-      </c>
-      <c r="E28" s="11">
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="11">
-        <v>0</v>
-      </c>
-      <c r="D29" s="11">
-        <v>0</v>
-      </c>
-      <c r="E29" s="11">
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="11">
-        <v>0</v>
-      </c>
-      <c r="D30" s="11">
-        <v>0</v>
-      </c>
-      <c r="E30" s="11">
+      <c r="C30" s="10">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="11">
-        <v>0</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0</v>
-      </c>
-      <c r="E31" s="11">
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="21.95" customHeight="1">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <f>SUM(C12:C31)</f>
         <v>12500</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="17">
         <f>SUM(D12:D31)</f>
         <v>16450</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="17">
         <f>SUM(E12:E31)</f>
         <v>16450</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="11.1" customHeight="1">
-      <c r="B33" s="19"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" ht="21.95" customHeight="1">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <f>C9-C32</f>
         <v>3000</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <f>D9-D32</f>
         <v>6050</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="10">
         <f>E9-E32</f>
         <v>6050</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21.95" customHeight="1">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10">
         <f>C34*0.2</f>
         <v>600</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="10">
         <f>D34*0.2</f>
         <v>1210</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="10">
         <f>E34*0.2</f>
         <v>1210</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="11.1" customHeight="1">
-      <c r="B36" s="19"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" ht="21.95" customHeight="1">
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="20">
         <f>C34-C35</f>
         <v>2400</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <f>D34-D35</f>
         <v>4840</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="20">
         <f>E34-E35</f>
         <v>4840</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="11.1" customHeight="1">
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" ht="21.95" customHeight="1">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="22">
         <f>C37</f>
         <v>2400</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="22">
         <f>D37</f>
         <v>4840</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="22">
         <f>E37</f>
         <v>4840</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5" ht="1.5" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="24"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="24"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25" t="s">
+      <c r="A43" s="23"/>
+      <c r="B43" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
     </row>
     <row r="44" spans="1:5" ht="36.950000000000003" customHeight="1">
-      <c r="A44" s="24"/>
-      <c r="B44" s="26" t="s">
+      <c r="A44" s="23"/>
+      <c r="B44" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1480,5 +1523,6 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>